<commit_message>
feat: simplify actual file
</commit_message>
<xml_diff>
--- a/tests/data/actual_default.xlsx
+++ b/tests/data/actual_default.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="8" mc:Ignorable="x14ac">
   <numFmts count="8">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
@@ -313,41 +313,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3">
+      <c r="B3" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>